<commit_message>
feat: new LSTM experiments
</commit_message>
<xml_diff>
--- a/LSTM/LSTM-Esperimenti/LSTM.xlsx
+++ b/LSTM/LSTM-Esperimenti/LSTM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24206"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_DC62435CA4BF603495C5ED4D73CEAADE5CF29AE1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2095AB0E-8426-41D5-BFEA-ED936737F7A6}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_DC62435CA4BF603495C5ED4D73CEAADE5CF29AE1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{249D9A23-39BE-4FE8-8352-50A1DD8566B8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="4">
   <si>
     <t>Prova n.</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>Layer</t>
   </si>
 </sst>
 </file>
@@ -1330,6 +1333,570 @@
         <a:ln w="0">
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>414</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>427</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9956759-88E7-4A50-9F30-D79C5060CE0B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="78981300"/>
+          <a:ext cx="6448425" cy="2447925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>414</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>427</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DA8AE4F-F6F9-4739-8033-84683303C0E6}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E9956759-88E7-4A50-9F30-D79C5060CE0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6877050" y="78924150"/>
+          <a:ext cx="3419475" cy="2371725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>429</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>448</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19F12CAF-218A-4FB2-AC48-BC363E685F83}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9DA8AE4F-F6F9-4739-8033-84683303C0E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="81667350"/>
+          <a:ext cx="10058400" cy="3800475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>450</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>469</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB7809FD-DD8B-4301-860F-A6E13556712A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{19F12CAF-218A-4FB2-AC48-BC363E685F83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="85667850"/>
+          <a:ext cx="10058400" cy="3752850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>475</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>488</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1445DD5-F973-47A8-A3D1-9553FB5E1FDB}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{EB7809FD-DD8B-4301-860F-A6E13556712A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="90439875"/>
+          <a:ext cx="6505575" cy="2466975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>474</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>487</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA015437-0CFB-430B-BF4D-1098911A5D46}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C1445DD5-F973-47A8-A3D1-9553FB5E1FDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6867525" y="90382725"/>
+          <a:ext cx="3419475" cy="2371725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>489</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>508</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8B2262C-7C41-4826-BEC5-2CA2A4A17518}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{CA015437-0CFB-430B-BF4D-1098911A5D46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="93097350"/>
+          <a:ext cx="10058400" cy="3800475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>510</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>529</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39DA8F3-3AE5-4490-9F2F-268E99813C61}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C8B2262C-7C41-4826-BEC5-2CA2A4A17518}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="97097850"/>
+          <a:ext cx="10058400" cy="3800475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>536</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>549</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C8C17C9-17A6-4F67-9BA4-C9B1807BEBF5}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E39DA8F3-3AE5-4490-9F2F-268E99813C61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="102098475"/>
+          <a:ext cx="6457950" cy="2447925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>535</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>548</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA82AA9-C41F-4B2A-9339-E3B1A66089AB}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7C8C17C9-17A6-4F67-9BA4-C9B1807BEBF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="102003225"/>
+          <a:ext cx="3419475" cy="2371725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>550</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>569</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0840BE48-3D10-4E36-87EA-A59F6278601C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4FA82AA9-C41F-4B2A-9339-E3B1A66089AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="104717850"/>
+          <a:ext cx="10058400" cy="3800475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>571</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>590</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{686DB76E-95F6-4E7D-B728-B2963F67B0B0}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{0840BE48-3D10-4E36-87EA-A59F6278601C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="108718350"/>
+          <a:ext cx="10058400" cy="3800475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1634,10 +2201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B350"/>
+  <dimension ref="A1:B535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="R353" sqref="R353:R354"/>
+    <sheetView tabSelected="1" topLeftCell="A540" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="L537" sqref="L537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -1834,7 +2401,87 @@
         <v>2</v>
       </c>
       <c r="B350" s="2">
-        <v>0.06</v>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2">
+      <c r="A412" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B412" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2">
+      <c r="A413" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B413" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2">
+      <c r="A414" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B414" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2">
+      <c r="A472" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B472" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2">
+      <c r="A473" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B473" s="2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2">
+      <c r="A474" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B474" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2">
+      <c r="A532" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B532" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2">
+      <c r="A533" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B533" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2">
+      <c r="A534" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B534" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2">
+      <c r="A535" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B535" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: update LSTM experiments
</commit_message>
<xml_diff>
--- a/LSTM/LSTM-Esperimenti/LSTM.xlsx
+++ b/LSTM/LSTM-Esperimenti/LSTM.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_DC62435CA4BF603495C5ED4D73CEAADE5CF29AE1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{249D9A23-39BE-4FE8-8352-50A1DD8566B8}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Tesi\LSTM\LSTM-Esperimenti\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF098257-071E-494F-9F9A-19F60F8A252A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training-Video" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="5">
   <si>
     <t>Prova n.</t>
   </si>
@@ -43,12 +48,15 @@
   <si>
     <t>Layer</t>
   </si>
+  <si>
+    <t>Finestra</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -104,7 +112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1901,11 +1909,411 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>596</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>383138</xdr:colOff>
+      <xdr:row>609</xdr:row>
+      <xdr:rowOff>34522</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Immagine 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5503C150-DD2C-40A2-A42A-46D79683D807}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="113623725"/>
+          <a:ext cx="6412463" cy="2425297"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>596</xdr:row>
+      <xdr:rowOff>101061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>609</xdr:row>
+      <xdr:rowOff>56755</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Immagine 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7F99894-9A42-4B2E-83F4-7814B17DB1FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6867525" y="113639061"/>
+          <a:ext cx="3448050" cy="2432194"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>611</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>346075</xdr:colOff>
+      <xdr:row>630</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Immagine 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94C53757-D35B-4B9C-9EC4-28548F48F71F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="116395500"/>
+          <a:ext cx="9804400" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>632</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>651</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Immagine 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9727C7DC-35A1-46F9-B96D-FB75A45ABC76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="120396000"/>
+          <a:ext cx="9753600" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>656</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>410612</xdr:colOff>
+      <xdr:row>669</xdr:row>
+      <xdr:rowOff>134822</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Immagine 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09E21079-7496-4F62-9EFF-AAB64F9F65F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="125139449"/>
+          <a:ext cx="6439937" cy="2439873"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>657</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>226190</xdr:colOff>
+      <xdr:row>669</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Immagine 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21611021-A476-4CAF-BA76-52DEB6D2E20B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6934200" y="125158501"/>
+          <a:ext cx="3321815" cy="2343150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>671</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>371735</xdr:colOff>
+      <xdr:row>690</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Immagine 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3244804-2E28-4866-AA72-DE40B7F9EDBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="127825500"/>
+          <a:ext cx="9830060" cy="3695700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>692</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>422273</xdr:colOff>
+      <xdr:row>711</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Immagine 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43F78439-8427-4E77-BC67-699AF2A6CA60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="131826000"/>
+          <a:ext cx="9880598" cy="3733800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2201,18 +2609,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B535"/>
+  <dimension ref="A1:B656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A540" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="L537" sqref="L537"/>
+    <sheetView tabSelected="1" topLeftCell="A652" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A693" sqref="A693"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2220,7 +2628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2228,7 +2636,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2236,7 +2644,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +2652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2252,7 +2660,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +2668,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -2268,7 +2676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
@@ -2276,7 +2684,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
@@ -2284,7 +2692,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
@@ -2292,7 +2700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>1</v>
       </c>
@@ -2300,7 +2708,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>2</v>
       </c>
@@ -2308,7 +2716,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>0</v>
       </c>
@@ -2316,7 +2724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>1</v>
       </c>
@@ -2324,7 +2732,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>2</v>
       </c>
@@ -2332,7 +2740,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>0</v>
       </c>
@@ -2340,7 +2748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>1</v>
       </c>
@@ -2348,7 +2756,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>2</v>
       </c>
@@ -2356,7 +2764,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>0</v>
       </c>
@@ -2364,7 +2772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>1</v>
       </c>
@@ -2372,7 +2780,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>2</v>
       </c>
@@ -2380,7 +2788,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="13.9">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>0</v>
       </c>
@@ -2388,7 +2796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="13.9">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>1</v>
       </c>
@@ -2396,7 +2804,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="13.9">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>2</v>
       </c>
@@ -2404,7 +2812,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="412" spans="1:2">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +2820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="413" spans="1:2">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>1</v>
       </c>
@@ -2420,7 +2828,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="414" spans="1:2">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>2</v>
       </c>
@@ -2428,7 +2836,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="472" spans="1:2">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" s="1" t="s">
         <v>0</v>
       </c>
@@ -2436,7 +2844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="473" spans="1:2">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" s="1" t="s">
         <v>1</v>
       </c>
@@ -2444,7 +2852,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="474" spans="1:2">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
         <v>2</v>
       </c>
@@ -2452,7 +2860,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="532" spans="1:2">
+    <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" s="1" t="s">
         <v>0</v>
       </c>
@@ -2460,7 +2868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="533" spans="1:2">
+    <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" s="1" t="s">
         <v>1</v>
       </c>
@@ -2468,7 +2876,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="534" spans="1:2">
+    <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" s="1" t="s">
         <v>2</v>
       </c>
@@ -2476,12 +2884,76 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="535" spans="1:2">
+    <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B535" s="2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A593" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B593" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A594" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B594" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A595" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B595" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A596" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B596" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A653" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B653" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A654" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B654" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B655" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B656" s="2">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2497,12 +2969,12 @@
   <sheetViews>
     <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2518,7 +2990,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>